<commit_message>
Update ci/cd and TestPerformance
</commit_message>
<xml_diff>
--- a/TourGuide/TourGuide_Performance_Graphs.xlsx
+++ b/TourGuide/TourGuide_Performance_Graphs.xlsx
@@ -1262,7 +1262,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1310,50 +1310,6 @@
         <v>1.0</v>
       </c>
       <c r="D3" t="n" s="1">
-        <v>900.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="n" s="1">
-        <v>5000.0</v>
-      </c>
-      <c r="C4" t="n" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="D4" t="n" s="1">
-        <v>900.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="n" s="1">
-        <v>10000.0</v>
-      </c>
-      <c r="C5" t="n" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="D5" t="n" s="1">
-        <v>900.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="n" s="1">
-        <v>50000.0</v>
-      </c>
-      <c r="C6" t="n" s="1">
-        <v>106.0</v>
-      </c>
-      <c r="D6" t="n" s="1">
-        <v>900.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="n" s="1">
-        <v>100000.0</v>
-      </c>
-      <c r="C7" t="n" s="1">
-        <v>212.0</v>
-      </c>
-      <c r="D7" t="n" s="1">
         <v>900.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add javadoc and reporting
</commit_message>
<xml_diff>
--- a/TourGuide/TourGuide_Performance_Graphs.xlsx
+++ b/TourGuide/TourGuide_Performance_Graphs.xlsx
@@ -1262,7 +1262,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1310,6 +1310,50 @@
         <v>1.0</v>
       </c>
       <c r="D3" t="n" s="1">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n" s="1">
+        <v>5000.0</v>
+      </c>
+      <c r="C4" t="n" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="D4" t="n" s="1">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n" s="1">
+        <v>10000.0</v>
+      </c>
+      <c r="C5" t="n" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="D5" t="n" s="1">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n" s="1">
+        <v>50000.0</v>
+      </c>
+      <c r="C6" t="n" s="1">
+        <v>105.0</v>
+      </c>
+      <c r="D6" t="n" s="1">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n" s="1">
+        <v>100000.0</v>
+      </c>
+      <c r="C7" t="n" s="1">
+        <v>212.0</v>
+      </c>
+      <c r="D7" t="n" s="1">
         <v>900.0</v>
       </c>
     </row>
@@ -1419,7 +1463,7 @@
         <v>100000.0</v>
       </c>
       <c r="C7" t="n" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7" t="n" s="1">
         <v>1200.0</v>

</xml_diff>